<commit_message>
this commit is to add homePage checkout and summary page file
</commit_message>
<xml_diff>
--- a/src/test/java/com/qkart/testData/LoginData.xlsx
+++ b/src/test/java/com/qkart/testData/LoginData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>userName</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>12test21</t>
-  </si>
-  <si>
-    <t>22test22</t>
   </si>
 </sst>
 </file>
@@ -357,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -381,14 +378,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>